<commit_message>
Loop spreadsheet entries and write to db
</commit_message>
<xml_diff>
--- a/input-data/publications-summary.xlsx
+++ b/input-data/publications-summary.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="200" windowWidth="27460" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="2014" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2014'!$A$3:$J$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2014'!$A$1:$J$53</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="167">
   <si>
     <t>URL</t>
   </si>
@@ -460,9 +460,6 @@
     <t>US$31.50; Policy note: Online access for 24 hours; see: http://www.nmd-journal.com/article/S0960-8966(13)00997-8/pdf</t>
   </si>
   <si>
-    <t>Source: PubMed; accessed 12 Jan 2015</t>
-  </si>
-  <si>
     <t>Cost (if applicable)</t>
   </si>
   <si>
@@ -530,16 +527,13 @@
   </si>
   <si>
     <t>PubMed says it's not available as free full text, but it's accessible through link in column I</t>
-  </si>
-  <si>
-    <t>PUBMED PUBLICATIONS ON FABRY DISEASE (2014)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,14 +562,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Trebuchet MS"/>
@@ -618,16 +604,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -636,7 +621,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -915,7 +900,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -923,73 +908,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.83203125" style="1"/>
     <col min="6" max="6" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44" style="3" customWidth="1"/>
-    <col min="8" max="8" width="54.5" style="10" customWidth="1"/>
+    <col min="8" max="8" width="54.5" style="9" customWidth="1"/>
     <col min="9" max="9" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="44.6640625" style="3" customWidth="1"/>
     <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="4" t="s">
-        <v>168</v>
+      <c r="A1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="65">
+      <c r="A2" s="1">
+        <v>25385939</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="A3" s="1">
+        <v>25345090</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="65">
       <c r="A4" s="1">
-        <v>25385939</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>5</v>
+        <v>25332282</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>33</v>
@@ -1001,9 +1045,9 @@
         <v>33</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H4" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -1013,15 +1057,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" ht="26">
       <c r="A5" s="1">
-        <v>25345090</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>6</v>
+        <v>25327101</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>34</v>
@@ -1035,28 +1079,28 @@
       <c r="G5" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>113</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="65">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="39">
       <c r="A6" s="1">
-        <v>25332282</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>7</v>
+        <v>25101867</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>34</v>
@@ -1065,9 +1109,9 @@
         <v>33</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="H6" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -1077,47 +1121,47 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="26">
+    <row r="7" spans="1:10" ht="27">
       <c r="A7" s="1">
-        <v>25327101</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>8</v>
+        <v>25073565</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>113</v>
+      <c r="H7" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="39">
       <c r="A8" s="1">
-        <v>25101867</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>9</v>
+        <v>25031264</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>34</v>
@@ -1129,9 +1173,9 @@
         <v>33</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H8" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -1141,15 +1185,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="27">
+    <row r="9" spans="1:10" ht="26">
       <c r="A9" s="1">
-        <v>25073565</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>10</v>
+        <v>24886109</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>34</v>
@@ -1163,57 +1207,57 @@
       <c r="G9" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>115</v>
+      <c r="I9" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="39">
+    <row r="10" spans="1:10" ht="52">
       <c r="A10" s="1">
-        <v>25031264</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>11</v>
+        <v>24823749</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>113</v>
+        <v>113</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>148</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>113</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="26">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="39">
       <c r="A11" s="1">
-        <v>24886109</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>12</v>
+        <v>24778057</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>34</v>
@@ -1222,65 +1266,65 @@
         <v>34</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>148</v>
+      <c r="H11" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>113</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="52">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="39">
       <c r="A12" s="1">
-        <v>24823749</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>13</v>
+        <v>24742848</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>149</v>
+        <v>164</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>113</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="39">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="26">
       <c r="A13" s="1">
-        <v>24778057</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>14</v>
+        <v>24738180</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>34</v>
@@ -1291,60 +1335,60 @@
       <c r="G13" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>113</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="39">
       <c r="A14" s="1">
-        <v>24742848</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>15</v>
+        <v>24724369</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G14" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="H14" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="26">
+    </row>
+    <row r="15" spans="1:10" ht="39">
       <c r="A15" s="1">
-        <v>24738180</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>16</v>
+        <v>24679964</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>34</v>
@@ -1355,57 +1399,57 @@
       <c r="G15" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>113</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="39">
       <c r="A16" s="1">
-        <v>24724369</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>17</v>
+        <v>24656905</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H16" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>113</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="39">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="26">
       <c r="A17" s="1">
-        <v>24679964</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>18</v>
+        <v>24640811</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>34</v>
@@ -1419,28 +1463,28 @@
       <c r="G17" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>113</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="39">
       <c r="A18" s="1">
-        <v>24656905</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>19</v>
+        <v>24632283</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>34</v>
@@ -1449,9 +1493,9 @@
         <v>33</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H18" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -1461,15 +1505,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="26">
+    <row r="19" spans="1:10" ht="27">
       <c r="A19" s="1">
-        <v>24640811</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>20</v>
+        <v>24626659</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>34</v>
@@ -1478,33 +1522,33 @@
         <v>34</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H19" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>113</v>
+      <c r="H19" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="39">
       <c r="A20" s="1">
-        <v>24632283</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>21</v>
+        <v>24613481</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>34</v>
@@ -1513,9 +1557,9 @@
         <v>33</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H20" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -1525,15 +1569,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="27">
+    <row r="21" spans="1:10" ht="39">
       <c r="A21" s="1">
-        <v>24626659</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>22</v>
+        <v>24582695</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>34</v>
@@ -1542,126 +1586,126 @@
         <v>34</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H21" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="65">
+      <c r="A22" s="1">
+        <v>24556355</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="65">
+      <c r="A23" s="1">
+        <v>24556354</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="14">
+      <c r="A24" s="1">
+        <v>24550428</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H24" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I24" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J21" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="39">
-      <c r="A22" s="1">
-        <v>24613481</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="39">
-      <c r="A23" s="1">
-        <v>24582695</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="65">
-      <c r="A24" s="1">
-        <v>24556355</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="J24" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="65">
+    <row r="25" spans="1:10" ht="39">
       <c r="A25" s="1">
-        <v>24556354</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>26</v>
+        <v>24534763</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>34</v>
@@ -1673,9 +1717,9 @@
         <v>33</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H25" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H25" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I25" s="1" t="s">
@@ -1685,18 +1729,18 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="14">
+    <row r="26" spans="1:10" ht="40">
       <c r="A26" s="1">
-        <v>24550428</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>27</v>
+        <v>24529306</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>34</v>
@@ -1707,10 +1751,10 @@
       <c r="G26" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H26" s="12" t="s">
+      <c r="H26" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="I26" s="7" t="s">
         <v>115</v>
       </c>
       <c r="J26" s="3" t="s">
@@ -1719,13 +1763,13 @@
     </row>
     <row r="27" spans="1:10" ht="39">
       <c r="A27" s="1">
-        <v>24534763</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>28</v>
+        <v>24513544</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>34</v>
@@ -1737,9 +1781,9 @@
         <v>33</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="H27" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H27" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -1749,15 +1793,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="40">
+    <row r="28" spans="1:10" ht="27">
       <c r="A28" s="1">
-        <v>24529306</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>29</v>
+        <v>24496231</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>34</v>
@@ -1771,25 +1815,25 @@
       <c r="G28" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="H28" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="I28" s="7" t="s">
         <v>115</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="39">
+    <row r="29" spans="1:10" ht="27">
       <c r="A29" s="1">
-        <v>24513544</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>30</v>
+        <v>24475221</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>34</v>
@@ -1798,16 +1842,16 @@
         <v>34</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>113</v>
+        <v>113</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>113</v>
@@ -1815,13 +1859,13 @@
     </row>
     <row r="30" spans="1:10" ht="27">
       <c r="A30" s="1">
-        <v>24496231</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>31</v>
+        <v>24398019</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>34</v>
@@ -1835,10 +1879,10 @@
       <c r="G30" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H30" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="I30" s="8" t="s">
+      <c r="H30" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I30" s="7" t="s">
         <v>115</v>
       </c>
       <c r="J30" s="3" t="s">
@@ -1847,13 +1891,13 @@
     </row>
     <row r="31" spans="1:10" ht="27">
       <c r="A31" s="1">
-        <v>24475221</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>50</v>
+        <v>24395922</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>34</v>
@@ -1862,30 +1906,30 @@
         <v>34</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H31" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="I31" s="8" t="s">
+      <c r="H31" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="I31" s="7" t="s">
         <v>115</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="27">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="39">
       <c r="A32" s="1">
-        <v>24398019</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>54</v>
+        <v>24380807</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>34</v>
@@ -1894,144 +1938,144 @@
         <v>34</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="I32" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="26">
+      <c r="A33" s="1">
+        <v>24365053</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="26">
+      <c r="A34" s="1">
+        <v>24361605</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="39">
+      <c r="A35" s="1">
+        <v>24341606</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="27">
+      <c r="A36" s="1">
+        <v>24335674</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I36" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="27">
-      <c r="A33" s="1">
-        <v>24395922</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H33" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="39">
-      <c r="A34" s="1">
-        <v>24380807</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="26">
-      <c r="A35" s="1">
-        <v>24365053</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H35" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="26">
-      <c r="A36" s="1">
-        <v>24361605</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="J36" s="3" t="s">
         <v>113</v>
@@ -2039,63 +2083,63 @@
     </row>
     <row r="37" spans="1:10" ht="39">
       <c r="A37" s="1">
-        <v>24341606</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>59</v>
+        <v>24334116</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H37" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H37" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>113</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="27">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="39">
       <c r="A38" s="1">
-        <v>24335674</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>60</v>
+        <v>24334114</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>115</v>
+        <v>123</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>113</v>
@@ -2103,16 +2147,16 @@
     </row>
     <row r="39" spans="1:10" ht="39">
       <c r="A39" s="1">
-        <v>24334116</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>61</v>
+        <v>24331397</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>34</v>
@@ -2121,9 +2165,9 @@
         <v>33</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H39" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H39" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I39" s="1" t="s">
@@ -2135,13 +2179,13 @@
     </row>
     <row r="40" spans="1:10" ht="39">
       <c r="A40" s="1">
-        <v>24334114</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>62</v>
+        <v>24239767</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>34</v>
@@ -2153,9 +2197,9 @@
         <v>33</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="H40" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="H40" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I40" s="1" t="s">
@@ -2165,47 +2209,47 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="39">
+    <row r="41" spans="1:10" ht="52">
       <c r="A41" s="1">
-        <v>24331397</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>63</v>
+        <v>24232002</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="H41" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="H41" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>113</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="39">
       <c r="A42" s="1">
-        <v>24239767</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>64</v>
+        <v>24215843</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>34</v>
@@ -2217,9 +2261,9 @@
         <v>33</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H42" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="H42" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I42" s="1" t="s">
@@ -2229,47 +2273,47 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="52">
+    <row r="43" spans="1:10" ht="26">
       <c r="A43" s="1">
-        <v>24232002</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>70</v>
+        <v>24196119</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="H43" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H43" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>113</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="39">
       <c r="A44" s="1">
-        <v>24215843</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>71</v>
+        <v>24189976</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>34</v>
@@ -2281,9 +2325,9 @@
         <v>33</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="H44" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H44" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I44" s="1" t="s">
@@ -2293,47 +2337,47 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="26">
+    <row r="45" spans="1:10" ht="27">
       <c r="A45" s="1">
-        <v>24196119</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>78</v>
+        <v>24158513</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H45" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>113</v>
+      <c r="H45" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="39">
       <c r="A46" s="1">
-        <v>24189976</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>79</v>
+        <v>24140492</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>34</v>
@@ -2345,9 +2389,9 @@
         <v>33</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H46" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H46" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I46" s="1" t="s">
@@ -2357,15 +2401,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="27">
+    <row r="47" spans="1:10" ht="39">
       <c r="A47" s="1">
-        <v>24158513</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>80</v>
+        <v>24129560</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>34</v>
@@ -2374,161 +2418,161 @@
         <v>34</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H47" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="52">
+      <c r="A48" s="1">
+        <v>24104692</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H48" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="52">
+      <c r="A49" s="1">
+        <v>24078459</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="39">
+      <c r="A50" s="1">
+        <v>23974650</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="40">
+      <c r="A51" s="1">
+        <v>23922385</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H51" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="I47" s="8" t="s">
+      <c r="I51" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J47" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="39">
-      <c r="A48" s="1">
-        <v>24140492</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="H48" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="39">
-      <c r="A49" s="1">
-        <v>24129560</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="H49" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="52">
-      <c r="A50" s="1">
-        <v>24104692</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H50" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="52">
-      <c r="A51" s="1">
-        <v>24078459</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="H51" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="J51" s="3" t="s">
-        <v>113</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="39">
       <c r="A52" s="1">
-        <v>23974650</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>90</v>
+        <v>23828401</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>34</v>
@@ -2537,9 +2581,9 @@
         <v>33</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="H52" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="H52" s="9" t="s">
         <v>113</v>
       </c>
       <c r="I52" s="1" t="s">
@@ -2549,15 +2593,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="40">
+    <row r="53" spans="1:10" ht="39">
       <c r="A53" s="1">
-        <v>23922385</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>91</v>
+        <v>23615762</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>34</v>
@@ -2569,168 +2613,99 @@
         <v>33</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H53" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="I53" s="8" t="s">
-        <v>115</v>
+        <v>136</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="39">
-      <c r="A54" s="1">
-        <v>23828401</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="H54" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J54" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="39">
-      <c r="A55" s="1">
-        <v>23615762</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H55" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J55" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
-      <c r="A57" s="1" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:J55"/>
+  <autoFilter ref="A1:J53"/>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B7" r:id="rId2"/>
-    <hyperlink ref="B8" r:id="rId3"/>
-    <hyperlink ref="B9" r:id="rId4"/>
-    <hyperlink ref="B10" r:id="rId5"/>
-    <hyperlink ref="B11" r:id="rId6"/>
-    <hyperlink ref="B13" r:id="rId7"/>
-    <hyperlink ref="B14" r:id="rId8"/>
-    <hyperlink ref="B15" r:id="rId9"/>
-    <hyperlink ref="B16" r:id="rId10"/>
-    <hyperlink ref="B17" r:id="rId11"/>
-    <hyperlink ref="B18" r:id="rId12"/>
-    <hyperlink ref="B19" r:id="rId13"/>
-    <hyperlink ref="B20" r:id="rId14"/>
-    <hyperlink ref="B21" r:id="rId15"/>
-    <hyperlink ref="B22" r:id="rId16"/>
-    <hyperlink ref="B23" r:id="rId17"/>
-    <hyperlink ref="B24" r:id="rId18"/>
-    <hyperlink ref="B25" r:id="rId19"/>
-    <hyperlink ref="B26" r:id="rId20"/>
-    <hyperlink ref="B27" r:id="rId21"/>
-    <hyperlink ref="B28" r:id="rId22"/>
-    <hyperlink ref="B29" r:id="rId23"/>
-    <hyperlink ref="B30" r:id="rId24"/>
-    <hyperlink ref="B31" r:id="rId25"/>
-    <hyperlink ref="B32" r:id="rId26"/>
-    <hyperlink ref="B33" r:id="rId27"/>
-    <hyperlink ref="B34" r:id="rId28"/>
-    <hyperlink ref="B35" r:id="rId29"/>
-    <hyperlink ref="B36" r:id="rId30"/>
-    <hyperlink ref="B37" r:id="rId31"/>
-    <hyperlink ref="B39" r:id="rId32"/>
-    <hyperlink ref="B40" r:id="rId33"/>
-    <hyperlink ref="B41" r:id="rId34"/>
-    <hyperlink ref="B42" r:id="rId35"/>
-    <hyperlink ref="B43" r:id="rId36"/>
-    <hyperlink ref="B44" r:id="rId37"/>
-    <hyperlink ref="B45" r:id="rId38"/>
-    <hyperlink ref="B46" r:id="rId39"/>
-    <hyperlink ref="B47" r:id="rId40"/>
-    <hyperlink ref="B48" r:id="rId41"/>
-    <hyperlink ref="B49" r:id="rId42"/>
-    <hyperlink ref="B50" r:id="rId43"/>
-    <hyperlink ref="B51" r:id="rId44"/>
-    <hyperlink ref="B53" r:id="rId45"/>
-    <hyperlink ref="B54" r:id="rId46"/>
-    <hyperlink ref="B55" r:id="rId47"/>
-    <hyperlink ref="B4" r:id="rId48"/>
-    <hyperlink ref="B5" r:id="rId49"/>
-    <hyperlink ref="I9" r:id="rId50"/>
-    <hyperlink ref="B12" r:id="rId51"/>
-    <hyperlink ref="I21" r:id="rId52"/>
-    <hyperlink ref="I26" r:id="rId53"/>
-    <hyperlink ref="I28" r:id="rId54"/>
-    <hyperlink ref="I30" r:id="rId55"/>
-    <hyperlink ref="I31" r:id="rId56"/>
-    <hyperlink ref="I32" r:id="rId57"/>
-    <hyperlink ref="B38" r:id="rId58"/>
-    <hyperlink ref="I38" r:id="rId59"/>
-    <hyperlink ref="I47" r:id="rId60"/>
-    <hyperlink ref="B52" r:id="rId61"/>
-    <hyperlink ref="I53" r:id="rId62"/>
-    <hyperlink ref="H9" r:id="rId63"/>
-    <hyperlink ref="H11" r:id="rId64"/>
-    <hyperlink ref="H12" r:id="rId65"/>
-    <hyperlink ref="H13" r:id="rId66" display="http://ar.iiarjournals.org/content/34/5/2437.full.pdf"/>
-    <hyperlink ref="H21" r:id="rId67"/>
-    <hyperlink ref="H26" r:id="rId68"/>
-    <hyperlink ref="H28" r:id="rId69"/>
-    <hyperlink ref="H30" r:id="rId70"/>
-    <hyperlink ref="H31" r:id="rId71"/>
-    <hyperlink ref="H32" r:id="rId72"/>
-    <hyperlink ref="H33" r:id="rId73"/>
-    <hyperlink ref="H36" r:id="rId74"/>
-    <hyperlink ref="H38" r:id="rId75"/>
-    <hyperlink ref="H47" r:id="rId76"/>
-    <hyperlink ref="H53" r:id="rId77"/>
-    <hyperlink ref="I33" r:id="rId78"/>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
+    <hyperlink ref="B9" r:id="rId6"/>
+    <hyperlink ref="B11" r:id="rId7"/>
+    <hyperlink ref="B12" r:id="rId8"/>
+    <hyperlink ref="B13" r:id="rId9"/>
+    <hyperlink ref="B14" r:id="rId10"/>
+    <hyperlink ref="B15" r:id="rId11"/>
+    <hyperlink ref="B16" r:id="rId12"/>
+    <hyperlink ref="B17" r:id="rId13"/>
+    <hyperlink ref="B18" r:id="rId14"/>
+    <hyperlink ref="B19" r:id="rId15"/>
+    <hyperlink ref="B20" r:id="rId16"/>
+    <hyperlink ref="B21" r:id="rId17"/>
+    <hyperlink ref="B22" r:id="rId18"/>
+    <hyperlink ref="B23" r:id="rId19"/>
+    <hyperlink ref="B24" r:id="rId20"/>
+    <hyperlink ref="B25" r:id="rId21"/>
+    <hyperlink ref="B26" r:id="rId22"/>
+    <hyperlink ref="B27" r:id="rId23"/>
+    <hyperlink ref="B28" r:id="rId24"/>
+    <hyperlink ref="B29" r:id="rId25"/>
+    <hyperlink ref="B30" r:id="rId26"/>
+    <hyperlink ref="B31" r:id="rId27"/>
+    <hyperlink ref="B32" r:id="rId28"/>
+    <hyperlink ref="B33" r:id="rId29"/>
+    <hyperlink ref="B34" r:id="rId30"/>
+    <hyperlink ref="B35" r:id="rId31"/>
+    <hyperlink ref="B37" r:id="rId32"/>
+    <hyperlink ref="B38" r:id="rId33"/>
+    <hyperlink ref="B39" r:id="rId34"/>
+    <hyperlink ref="B40" r:id="rId35"/>
+    <hyperlink ref="B41" r:id="rId36"/>
+    <hyperlink ref="B42" r:id="rId37"/>
+    <hyperlink ref="B43" r:id="rId38"/>
+    <hyperlink ref="B44" r:id="rId39"/>
+    <hyperlink ref="B45" r:id="rId40"/>
+    <hyperlink ref="B46" r:id="rId41"/>
+    <hyperlink ref="B47" r:id="rId42"/>
+    <hyperlink ref="B48" r:id="rId43"/>
+    <hyperlink ref="B49" r:id="rId44"/>
+    <hyperlink ref="B51" r:id="rId45"/>
+    <hyperlink ref="B52" r:id="rId46"/>
+    <hyperlink ref="B53" r:id="rId47"/>
+    <hyperlink ref="B2" r:id="rId48"/>
+    <hyperlink ref="B3" r:id="rId49"/>
+    <hyperlink ref="I7" r:id="rId50"/>
+    <hyperlink ref="B10" r:id="rId51"/>
+    <hyperlink ref="I19" r:id="rId52"/>
+    <hyperlink ref="I24" r:id="rId53"/>
+    <hyperlink ref="I26" r:id="rId54"/>
+    <hyperlink ref="I28" r:id="rId55"/>
+    <hyperlink ref="I29" r:id="rId56"/>
+    <hyperlink ref="I30" r:id="rId57"/>
+    <hyperlink ref="B36" r:id="rId58"/>
+    <hyperlink ref="I36" r:id="rId59"/>
+    <hyperlink ref="I45" r:id="rId60"/>
+    <hyperlink ref="B50" r:id="rId61"/>
+    <hyperlink ref="I51" r:id="rId62"/>
+    <hyperlink ref="H7" r:id="rId63"/>
+    <hyperlink ref="H9" r:id="rId64"/>
+    <hyperlink ref="H10" r:id="rId65"/>
+    <hyperlink ref="H11" r:id="rId66" display="http://ar.iiarjournals.org/content/34/5/2437.full.pdf"/>
+    <hyperlink ref="H19" r:id="rId67"/>
+    <hyperlink ref="H24" r:id="rId68"/>
+    <hyperlink ref="H26" r:id="rId69"/>
+    <hyperlink ref="H28" r:id="rId70"/>
+    <hyperlink ref="H29" r:id="rId71"/>
+    <hyperlink ref="H30" r:id="rId72"/>
+    <hyperlink ref="H31" r:id="rId73"/>
+    <hyperlink ref="H34" r:id="rId74"/>
+    <hyperlink ref="H36" r:id="rId75"/>
+    <hyperlink ref="H45" r:id="rId76"/>
+    <hyperlink ref="H51" r:id="rId77"/>
+    <hyperlink ref="I31" r:id="rId78"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>